<commit_message>
finished to question 6
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary van Valkenburg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\Documents\DA11\Excel\lookups-exercise-Timothyspratt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6144008E-EB49-430B-8F1B-A1A64E552A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="90" windowWidth="21877" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13665" yWindow="0" windowWidth="24735" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -314,7 +314,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,7 +458,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1176,13 +1176,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P107"/>
+  <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
@@ -1196,7 +1196,7 @@
     <col min="16" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1256,23 +1256,56 @@
       <c r="C2">
         <v>341243679.13</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="D2">
+        <f>B2-C2</f>
+        <v>15396420.870000005</v>
+      </c>
+      <c r="E2" s="5">
+        <f>IFERROR(D2/B2,0)</f>
+        <v>4.3170750765267295E-2</v>
+      </c>
+      <c r="F2">
+        <f>RANK(E2,E2:E52)</f>
+        <v>14</v>
+      </c>
       <c r="G2">
         <v>382685200</v>
       </c>
       <c r="H2">
         <v>346340810.81999999</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="I2">
+        <f>G2-H2</f>
+        <v>36344389.180000007</v>
+      </c>
+      <c r="J2" s="5">
+        <f>IFERROR(I2/G2,0)</f>
+        <v>9.4972027086493035E-2</v>
+      </c>
+      <c r="K2">
+        <f>RANK(J2,J2:J52)</f>
+        <v>10</v>
+      </c>
       <c r="L2">
         <v>376548600</v>
       </c>
       <c r="M2">
         <v>355279492.22999901</v>
       </c>
-      <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="N2">
+        <f>L2-M2</f>
+        <v>21269107.770000994</v>
+      </c>
+      <c r="O2" s="5">
+        <f>IFERROR(N2/L2,0)</f>
+        <v>5.6484362894991494E-2</v>
+      </c>
+      <c r="P2">
+        <f>RANK(O2,O2:O52)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1282,23 +1315,56 @@
       <c r="C3">
         <v>321214.59000000003</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="D3">
+        <f t="shared" ref="D3:D52" si="0">B3-C3</f>
+        <v>7585.4099999999744</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E52" si="1">IFERROR(D3/B3,0)</f>
+        <v>2.3069981751824741E-2</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F52" si="2">RANK(E3,E3:E53)</f>
+        <v>21</v>
+      </c>
       <c r="G3">
         <v>334800</v>
       </c>
       <c r="H3">
         <v>312433.70999999897</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="I3">
+        <f t="shared" ref="I3:I52" si="3">G3-H3</f>
+        <v>22366.290000001027</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" ref="J3:J52" si="4">IFERROR(I3/G3,0)</f>
+        <v>6.6804928315415249E-2</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K52" si="5">RANK(J3,J3:J53)</f>
+        <v>13</v>
+      </c>
       <c r="L3">
         <v>322700</v>
       </c>
       <c r="M3">
         <v>322263.03999999998</v>
       </c>
-      <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="N3">
+        <f t="shared" ref="N3:N52" si="6">L3-M3</f>
+        <v>436.96000000002095</v>
+      </c>
+      <c r="O3" s="5">
+        <f t="shared" ref="O3:O52" si="7">IFERROR(N3/L3,0)</f>
+        <v>1.3540749922529313E-3</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P52" si="8">RANK(O3,O3:O53)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1308,23 +1374,56 @@
       <c r="C4">
         <v>3115157.5599999898</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>15442.440000010189</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="1"/>
+        <v>4.9327413275443007E-3</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
       <c r="G4">
         <v>3652300</v>
       </c>
       <c r="H4">
         <v>3589693.2099999902</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>62606.790000009816</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" si="4"/>
+        <v>1.7141743558856015E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
       <c r="L4">
         <v>3662400</v>
       </c>
       <c r="M4">
         <v>3564983.04999999</v>
       </c>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="N4">
+        <f t="shared" si="6"/>
+        <v>97416.950000009965</v>
+      </c>
+      <c r="O4" s="5">
+        <f t="shared" si="7"/>
+        <v>2.6599210899959033E-2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1334,23 +1433,56 @@
       <c r="C5">
         <v>6947552.6699999999</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>723147.33000000007</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
+        <v>9.4273968477453174E-2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
       <c r="G5">
         <v>7968300</v>
       </c>
       <c r="H5">
         <v>7020609.3200000003</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>947690.6799999997</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="4"/>
+        <v>0.118932605449092</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
       <c r="L5">
         <v>7759600</v>
       </c>
       <c r="M5">
         <v>7497322.9100000001</v>
       </c>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="N5">
+        <f t="shared" si="6"/>
+        <v>262277.08999999985</v>
+      </c>
+      <c r="O5" s="5">
+        <f t="shared" si="7"/>
+        <v>3.3800336357544182E-2</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="8"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1360,23 +1492,56 @@
       <c r="C6">
         <v>385908.52</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>23391.479999999981</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>5.7149963352064452E-2</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
       <c r="G6">
         <v>428500</v>
       </c>
       <c r="H6">
         <v>427758.64</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>741.35999999998603</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="4"/>
+        <v>1.7301283547257551E-3</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
       <c r="L6">
         <v>445200</v>
       </c>
       <c r="M6">
         <v>445114.28999999899</v>
       </c>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="N6">
+        <f t="shared" si="6"/>
+        <v>85.710000001010485</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="shared" si="7"/>
+        <v>1.925202156356929E-4</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1386,23 +1551,56 @@
       <c r="C7">
         <v>2946071.21</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>382928.79000000004</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.11502817362571344</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="G7">
         <v>3390900</v>
       </c>
       <c r="H7">
         <v>3051483.41</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>339416.58999999985</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="4"/>
+        <v>0.10009631366303927</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
       <c r="L7">
         <v>3345200</v>
       </c>
       <c r="M7">
         <v>2946440.08</v>
       </c>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="N7">
+        <f t="shared" si="6"/>
+        <v>398759.91999999993</v>
+      </c>
+      <c r="O7" s="5">
+        <f t="shared" si="7"/>
+        <v>0.11920361114432618</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1412,23 +1610,56 @@
       <c r="C8">
         <v>1315623.30999999</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>236476.69000000996</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>0.15235918433091292</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="G8">
         <v>1590700</v>
       </c>
       <c r="H8">
         <v>1383905.98999999</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>206794.01000001002</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="4"/>
+        <v>0.13000189224870184</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
       <c r="L8">
         <v>1579300</v>
       </c>
       <c r="M8">
         <v>1337735.3199999901</v>
       </c>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="N8">
+        <f t="shared" si="6"/>
+        <v>241564.68000000995</v>
+      </c>
+      <c r="O8" s="5">
+        <f t="shared" si="7"/>
+        <v>0.15295680364719175</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1438,23 +1669,56 @@
       <c r="C9">
         <v>8952825.2799999993</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>396574.72000000067</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>4.2417130511048909E-2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
       <c r="G9">
         <v>11073700</v>
       </c>
       <c r="H9">
         <v>9929059.5199999996</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>1144640.4800000004</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="4"/>
+        <v>0.10336567542917005</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
       <c r="L9">
         <v>10790500</v>
       </c>
       <c r="M9">
         <v>9993599.52999999</v>
       </c>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="N9">
+        <f t="shared" si="6"/>
+        <v>796900.47000000998</v>
+      </c>
+      <c r="O9" s="5">
+        <f t="shared" si="7"/>
+        <v>7.3852043000788653E-2</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1464,23 +1728,56 @@
       <c r="C10">
         <v>407090.37</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>36209.630000000005</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>8.1681998646514792E-2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
       <c r="G10">
         <v>495200</v>
       </c>
       <c r="H10">
         <v>467907.84000000003</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>27292.159999999974</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="4"/>
+        <v>5.5113408723747932E-2</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
       <c r="L10">
         <v>487500</v>
       </c>
       <c r="M10">
         <v>478318.92</v>
       </c>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="N10">
+        <f t="shared" si="6"/>
+        <v>9181.0800000000163</v>
+      </c>
+      <c r="O10" s="5">
+        <f t="shared" si="7"/>
+        <v>1.883298461538465E-2</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1490,23 +1787,56 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
       <c r="L11">
         <v>375000</v>
       </c>
       <c r="M11">
         <v>63771.91</v>
       </c>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="N11">
+        <f t="shared" si="6"/>
+        <v>311228.08999999997</v>
+      </c>
+      <c r="O11" s="5">
+        <f t="shared" si="7"/>
+        <v>0.82994157333333329</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1516,23 +1846,56 @@
       <c r="C12">
         <v>4066595.33</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>214304.66999999993</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>5.0060657805601608E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
       <c r="G12">
         <v>4700400</v>
       </c>
       <c r="H12">
         <v>4205555.5999999996</v>
       </c>
-      <c r="J12" s="5"/>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>494844.40000000037</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="4"/>
+        <v>0.10527708280146378</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
       <c r="L12">
         <v>4677800</v>
       </c>
       <c r="M12">
         <v>4371713.1399999997</v>
       </c>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="N12">
+        <f t="shared" si="6"/>
+        <v>306086.86000000034</v>
+      </c>
+      <c r="O12" s="5">
+        <f t="shared" si="7"/>
+        <v>6.5433934755654441E-2</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1542,23 +1905,56 @@
       <c r="C13">
         <v>5772288.3300000001</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>75511.669999999925</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2912833886247806E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
       <c r="G13">
         <v>6223700</v>
       </c>
       <c r="H13">
         <v>5909077.9399999902</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>314622.06000000983</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="4"/>
+        <v>5.0552253482656594E-2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="L13">
         <v>6207300</v>
       </c>
       <c r="M13">
         <v>6056976.6699999999</v>
       </c>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="N13">
+        <f t="shared" si="6"/>
+        <v>150323.33000000007</v>
+      </c>
+      <c r="O13" s="5">
+        <f t="shared" si="7"/>
+        <v>2.4217184605222895E-2</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1568,23 +1964,56 @@
       <c r="C14">
         <v>505017.37</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>6982.6300000000047</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3637949218750009E-2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
       <c r="G14">
         <v>530500</v>
       </c>
       <c r="H14">
         <v>524402.98</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>6097.0200000000186</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="4"/>
+        <v>1.1492968897266765E-2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
       <c r="L14">
         <v>526200</v>
       </c>
       <c r="M14">
         <v>504989.88</v>
       </c>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="N14">
+        <f t="shared" si="6"/>
+        <v>21210.119999999995</v>
+      </c>
+      <c r="O14" s="5">
+        <f t="shared" si="7"/>
+        <v>4.0308095781071827E-2</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1594,23 +2023,56 @@
       <c r="C15">
         <v>156545919.90000001</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-496819.90000000596</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
+        <v>-3.1837408866824991E-3</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
       <c r="G15">
         <v>184167800</v>
       </c>
       <c r="H15">
         <v>175966389.24999899</v>
       </c>
-      <c r="J15" s="5"/>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>8201410.7500010133</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="4"/>
+        <v>4.4532273014072019E-2</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
       <c r="L15">
         <v>188953500</v>
       </c>
       <c r="M15">
         <v>184450910.84999901</v>
       </c>
-      <c r="O15" s="5"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="N15">
+        <f t="shared" si="6"/>
+        <v>4502589.1500009894</v>
+      </c>
+      <c r="O15" s="5">
+        <f t="shared" si="7"/>
+        <v>2.3829085727446114E-2</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1620,23 +2082,56 @@
       <c r="C16">
         <v>6522480.4599999897</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>78219.540000010282</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="1"/>
+        <v>1.1850188616360429E-2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
       <c r="G16">
         <v>7352500</v>
       </c>
       <c r="H16">
         <v>7350464.0800000001</v>
       </c>
-      <c r="J16" s="5"/>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>2035.9199999999255</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" si="4"/>
+        <v>2.769017341040361E-4</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
       <c r="L16">
         <v>7397200</v>
       </c>
       <c r="M16">
         <v>7397093</v>
       </c>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="N16">
+        <f t="shared" si="6"/>
+        <v>107</v>
+      </c>
+      <c r="O16" s="5">
+        <f t="shared" si="7"/>
+        <v>1.4464932677229222E-5</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1646,23 +2141,56 @@
       <c r="C17">
         <v>14439480.050000001</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>421319.94999999925</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="1"/>
+        <v>2.8351094826658003E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
       <c r="G17">
         <v>15309700</v>
       </c>
       <c r="H17">
         <v>14645233.51</v>
       </c>
-      <c r="J17" s="5"/>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>664466.49000000022</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" si="4"/>
+        <v>4.3401666263871937E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
       <c r="L17">
         <v>15311800</v>
       </c>
       <c r="M17">
         <v>14346057.039999999</v>
       </c>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="N17">
+        <f t="shared" si="6"/>
+        <v>965742.96000000089</v>
+      </c>
+      <c r="O17" s="5">
+        <f t="shared" si="7"/>
+        <v>6.3071811282801551E-2</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1672,23 +2200,56 @@
       <c r="C18">
         <v>2615303.8999999901</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>149396.10000000987</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
+        <v>5.4037002206391245E-2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
       <c r="G18">
         <v>2861000</v>
       </c>
       <c r="H18">
         <v>2671745.94</v>
       </c>
-      <c r="J18" s="5"/>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>189254.06000000006</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="4"/>
+        <v>6.6149619014330668E-2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
       <c r="L18">
         <v>2910600</v>
       </c>
       <c r="M18">
         <v>2535637.09</v>
       </c>
-      <c r="O18" s="5"/>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="N18">
+        <f t="shared" si="6"/>
+        <v>374962.91000000015</v>
+      </c>
+      <c r="O18" s="5">
+        <f t="shared" si="7"/>
+        <v>0.12882667147667154</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1698,23 +2259,56 @@
       <c r="C19">
         <v>8460963.1999999899</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>376336.80000001006</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="1"/>
+        <v>4.258504294298146E-2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
       <c r="G19">
         <v>9713300</v>
       </c>
       <c r="H19">
         <v>8991707.2399999909</v>
       </c>
-      <c r="J19" s="5"/>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>721592.76000000909</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" si="4"/>
+        <v>7.4289145810384635E-2</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
       <c r="L19">
         <v>9343000</v>
       </c>
       <c r="M19">
         <v>8766655.9100000001</v>
       </c>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="N19">
+        <f t="shared" si="6"/>
+        <v>576344.08999999985</v>
+      </c>
+      <c r="O19" s="5">
+        <f t="shared" si="7"/>
+        <v>6.1687262121374278E-2</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1724,23 +2318,56 @@
       <c r="C20">
         <v>124384360.159999</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1539.8400010019541</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2379538203300809E-5</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
       <c r="G20">
         <v>131849400</v>
       </c>
       <c r="H20">
         <v>131839624.37</v>
       </c>
-      <c r="J20" s="5"/>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>9775.6299999952316</v>
+      </c>
+      <c r="J20" s="5">
+        <f t="shared" si="4"/>
+        <v>7.4142392760188761E-5</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
       <c r="L20">
         <v>130621400</v>
       </c>
       <c r="M20">
         <v>130621283.53999899</v>
       </c>
-      <c r="O20" s="5"/>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="N20">
+        <f t="shared" si="6"/>
+        <v>116.46000100672245</v>
+      </c>
+      <c r="O20" s="5">
+        <f t="shared" si="7"/>
+        <v>8.9158438821450736E-7</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="8"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1750,23 +2377,56 @@
       <c r="C21">
         <v>22408587.5499999</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1923512.4500000998</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="1"/>
+        <v>7.9052463618023094E-2</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
       <c r="G21">
         <v>24497400</v>
       </c>
       <c r="H21">
         <v>22655993.629999999</v>
       </c>
-      <c r="J21" s="5"/>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>1841406.370000001</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" si="4"/>
+        <v>7.5167420624229556E-2</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
       <c r="L21">
         <v>24323000</v>
       </c>
       <c r="M21">
         <v>23434073.089999899</v>
       </c>
-      <c r="O21" s="5"/>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="N21">
+        <f t="shared" si="6"/>
+        <v>888926.91000010073</v>
+      </c>
+      <c r="O21" s="5">
+        <f t="shared" si="7"/>
+        <v>3.6546762734864152E-2</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1776,23 +2436,56 @@
       <c r="C22">
         <v>11412339.8799999</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>153660.12000009976</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3285502334437123E-2</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
       <c r="G22">
         <v>11980700</v>
       </c>
       <c r="H22">
         <v>11791977.9699999</v>
       </c>
-      <c r="J22" s="5"/>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>188722.03000009991</v>
+      </c>
+      <c r="J22" s="5">
+        <f t="shared" si="4"/>
+        <v>1.5752170574348738E-2</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
       <c r="L22">
         <v>11935200</v>
       </c>
       <c r="M22">
         <v>11934454.77</v>
       </c>
-      <c r="O22" s="5"/>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="N22">
+        <f t="shared" si="6"/>
+        <v>745.23000000044703</v>
+      </c>
+      <c r="O22" s="5">
+        <f t="shared" si="7"/>
+        <v>6.2439674240938325E-5</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1802,23 +2495,56 @@
       <c r="C23">
         <v>20036743.4099999</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>825956.59000010043</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>3.9590110100806722E-2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
       <c r="G23">
         <v>22683800</v>
       </c>
       <c r="H23">
         <v>21722126.219999898</v>
       </c>
-      <c r="J23" s="5"/>
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>961673.78000010177</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" si="4"/>
+        <v>4.2394738976719144E-2</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
       <c r="L23">
         <v>23220300</v>
       </c>
       <c r="M23">
         <v>22619057.440000001</v>
       </c>
-      <c r="O23" s="5"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="N23">
+        <f t="shared" si="6"/>
+        <v>601242.55999999866</v>
+      </c>
+      <c r="O23" s="5">
+        <f t="shared" si="7"/>
+        <v>2.5892971236375011E-2</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1828,23 +2554,56 @@
       <c r="C24">
         <v>904969.19</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>12230.810000000056</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3334943305713101E-2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
       <c r="G24">
         <v>1112700</v>
       </c>
       <c r="H24">
         <v>1067214.42</v>
       </c>
-      <c r="J24" s="5"/>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>45485.580000000075</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" si="4"/>
+        <v>4.087856565111897E-2</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
       <c r="L24">
         <v>1112600</v>
       </c>
       <c r="M24">
         <v>1112527.1200000001</v>
       </c>
-      <c r="O24" s="5"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="N24">
+        <f t="shared" si="6"/>
+        <v>72.879999999888241</v>
+      </c>
+      <c r="O24" s="5">
+        <f t="shared" si="7"/>
+        <v>6.5504224339284781E-5</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1854,23 +2613,56 @@
       <c r="C25">
         <v>479149.53</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>4950.4699999999721</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="1"/>
+        <v>1.0226130964676661E-2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
       <c r="G25">
         <v>505200</v>
       </c>
       <c r="H25">
         <v>497194.20999999897</v>
       </c>
-      <c r="J25" s="5"/>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>8005.7900000010268</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" si="4"/>
+        <v>1.5846773555029746E-2</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
       <c r="L25">
         <v>496500</v>
       </c>
       <c r="M25">
         <v>494775.1</v>
       </c>
-      <c r="O25" s="5"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="N25">
+        <f t="shared" si="6"/>
+        <v>1724.9000000000233</v>
+      </c>
+      <c r="O25" s="5">
+        <f t="shared" si="7"/>
+        <v>3.4741188318228064E-3</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1880,23 +2672,56 @@
       <c r="C26">
         <v>4801960.08</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>447839.91999999993</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="1"/>
+        <v>8.5306091660634673E-2</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="G26">
         <v>5442200</v>
       </c>
       <c r="H26">
         <v>5122329.02999999</v>
       </c>
-      <c r="J26" s="5"/>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>319870.97000000998</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" si="4"/>
+        <v>5.8776040939327839E-2</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
       <c r="L26">
         <v>5430700</v>
       </c>
       <c r="M26">
         <v>5117235.21</v>
       </c>
-      <c r="O26" s="5"/>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="N26">
+        <f t="shared" si="6"/>
+        <v>313464.79000000004</v>
+      </c>
+      <c r="O26" s="5">
+        <f t="shared" si="7"/>
+        <v>5.7720881286022069E-2</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1906,23 +2731,56 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="J27" s="5"/>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
-      <c r="O27" s="5"/>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="N27">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1932,23 +2790,56 @@
       <c r="C28">
         <v>1250442.02</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>132457.97999999998</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="1"/>
+        <v>9.5782760864849215E-2</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="G28">
         <v>1545700</v>
       </c>
       <c r="H28">
         <v>1281335.23</v>
       </c>
-      <c r="J28" s="5"/>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>264364.77</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" si="4"/>
+        <v>0.17103239309050916</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
       <c r="L28">
         <v>1525900</v>
       </c>
       <c r="M28">
         <v>1393285.06</v>
       </c>
-      <c r="O28" s="5"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="N28">
+        <f t="shared" si="6"/>
+        <v>132614.93999999994</v>
+      </c>
+      <c r="O28" s="5">
+        <f t="shared" si="7"/>
+        <v>8.6909325643882263E-2</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1958,23 +2849,56 @@
       <c r="C29">
         <v>2523884.71</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>37915.290000000037</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" si="1"/>
+        <v>1.4800253727847622E-2</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
       <c r="G29">
         <v>2779500</v>
       </c>
       <c r="H29">
         <v>2665264.4399999902</v>
       </c>
-      <c r="J29" s="5"/>
+      <c r="I29">
+        <f t="shared" si="3"/>
+        <v>114235.56000000983</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" si="4"/>
+        <v>4.1099320021590155E-2</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="L29">
         <v>2889900</v>
       </c>
       <c r="M29">
         <v>2889864.67</v>
       </c>
-      <c r="O29" s="5"/>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="N29">
+        <f t="shared" si="6"/>
+        <v>35.330000000074506</v>
+      </c>
+      <c r="O29" s="5">
+        <f t="shared" si="7"/>
+        <v>1.2225336516860273E-5</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1984,23 +2908,56 @@
       <c r="C30">
         <v>12030494.1</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>101705.90000000037</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="1"/>
+        <v>8.3831374359143746E-3</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
       <c r="G30">
         <v>12735900</v>
       </c>
       <c r="H30">
         <v>12685514.279999901</v>
       </c>
-      <c r="J30" s="5"/>
+      <c r="I30">
+        <f t="shared" si="3"/>
+        <v>50385.720000099391</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" si="4"/>
+        <v>3.9561962641116366E-3</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
       <c r="L30">
         <v>12861300</v>
       </c>
       <c r="M30">
         <v>12826009.609999999</v>
       </c>
-      <c r="O30" s="5"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="N30">
+        <f t="shared" si="6"/>
+        <v>35290.390000000596</v>
+      </c>
+      <c r="O30" s="5">
+        <f t="shared" si="7"/>
+        <v>2.7439209100169185E-3</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2010,23 +2967,56 @@
       <c r="C31">
         <v>1740827.69</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>24772.310000000056</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="1"/>
+        <v>1.4030533529678329E-2</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
       <c r="G31">
         <v>1823300</v>
       </c>
       <c r="H31">
         <v>1762676.85</v>
       </c>
-      <c r="J31" s="5"/>
+      <c r="I31">
+        <f t="shared" si="3"/>
+        <v>60623.149999999907</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" si="4"/>
+        <v>3.3249136181648611E-2</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
       <c r="L31">
         <v>1870700</v>
       </c>
       <c r="M31">
         <v>1801391.34</v>
       </c>
-      <c r="O31" s="5"/>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="N31">
+        <f t="shared" si="6"/>
+        <v>69308.659999999916</v>
+      </c>
+      <c r="O31" s="5">
+        <f t="shared" si="7"/>
+        <v>3.7049585716576634E-2</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2036,23 +3026,56 @@
       <c r="C32">
         <v>5925637.7199999904</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>73762.280000009574</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2294942827617691E-2</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
       <c r="G32">
         <v>6195500</v>
       </c>
       <c r="H32">
         <v>6084985.4699999997</v>
       </c>
-      <c r="J32" s="5"/>
+      <c r="I32">
+        <f t="shared" si="3"/>
+        <v>110514.53000000026</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" si="4"/>
+        <v>1.7837871035428981E-2</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
       <c r="L32">
         <v>6157400</v>
       </c>
       <c r="M32">
         <v>5987572.0199999996</v>
       </c>
-      <c r="O32" s="5"/>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="N32">
+        <f t="shared" si="6"/>
+        <v>169827.98000000045</v>
+      </c>
+      <c r="O32" s="5">
+        <f t="shared" si="7"/>
+        <v>2.7581118653977402E-2</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -2062,23 +3085,56 @@
       <c r="C33">
         <v>920284264.73000002</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>7418835.2699990273</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" si="1"/>
+        <v>7.9969930789269058E-3</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
       <c r="G33">
         <v>979671000</v>
       </c>
       <c r="H33">
         <v>977068513.48000002</v>
       </c>
-      <c r="J33" s="5"/>
+      <c r="I33">
+        <f t="shared" si="3"/>
+        <v>2602486.5199999809</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" si="4"/>
+        <v>2.6564903115433454E-3</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
       <c r="L33">
         <v>989572899.99999905</v>
       </c>
       <c r="M33">
         <v>984116289.40999901</v>
       </c>
-      <c r="O33" s="5"/>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="N33">
+        <f t="shared" si="6"/>
+        <v>5456610.5900000334</v>
+      </c>
+      <c r="O33" s="5">
+        <f t="shared" si="7"/>
+        <v>5.5141067323084929E-3</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2088,23 +3144,56 @@
       <c r="C34">
         <v>4109958.22</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>79341.779999999795</v>
+      </c>
+      <c r="E34" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8939149738619768E-2</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
       <c r="G34">
         <v>4350600</v>
       </c>
       <c r="H34">
         <v>4137588.7699999898</v>
       </c>
-      <c r="J34" s="5"/>
+      <c r="I34">
+        <f t="shared" si="3"/>
+        <v>213011.23000001023</v>
+      </c>
+      <c r="J34" s="5">
+        <f t="shared" si="4"/>
+        <v>4.8961345561534093E-2</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
       <c r="L34">
         <v>4345600</v>
       </c>
       <c r="M34">
         <v>4229801.51</v>
       </c>
-      <c r="O34" s="5"/>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="N34">
+        <f t="shared" si="6"/>
+        <v>115798.49000000022</v>
+      </c>
+      <c r="O34" s="5">
+        <f t="shared" si="7"/>
+        <v>2.6647296115611244E-2</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2114,23 +3203,56 @@
       <c r="C35">
         <v>0</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
-      <c r="J35" s="5"/>
+      <c r="I35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
         <v>0</v>
       </c>
-      <c r="O35" s="5"/>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="N35">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -2140,23 +3262,56 @@
       <c r="C36">
         <v>735423.27999999898</v>
       </c>
-      <c r="E36" s="5"/>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>62776.72000000102</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" si="1"/>
+        <v>7.8647857679780775E-2</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
       <c r="G36">
         <v>898700</v>
       </c>
       <c r="H36">
         <v>740966.94999999902</v>
       </c>
-      <c r="J36" s="5"/>
+      <c r="I36">
+        <f t="shared" si="3"/>
+        <v>157733.05000000098</v>
+      </c>
+      <c r="J36" s="5">
+        <f t="shared" si="4"/>
+        <v>0.17551246244575608</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
       <c r="L36">
         <v>878300</v>
       </c>
       <c r="M36">
         <v>777215.28999999899</v>
       </c>
-      <c r="O36" s="5"/>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="N36">
+        <f t="shared" si="6"/>
+        <v>101084.71000000101</v>
+      </c>
+      <c r="O36" s="5">
+        <f t="shared" si="7"/>
+        <v>0.11509132414892521</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2166,23 +3321,56 @@
       <c r="C37">
         <v>2005447.73999999</v>
       </c>
-      <c r="E37" s="5"/>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>82352.260000010021</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" si="1"/>
+        <v>3.9444515758219188E-2</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
       <c r="G37">
         <v>2229200</v>
       </c>
       <c r="H37">
         <v>2118943.21</v>
       </c>
-      <c r="J37" s="5"/>
+      <c r="I37">
+        <f t="shared" si="3"/>
+        <v>110256.79000000004</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" si="4"/>
+        <v>4.9460250314014013E-2</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
       <c r="L37">
         <v>2296900</v>
       </c>
       <c r="M37">
         <v>2108718.34</v>
       </c>
-      <c r="O37" s="5"/>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="N37">
+        <f t="shared" si="6"/>
+        <v>188181.66000000015</v>
+      </c>
+      <c r="O37" s="5">
+        <f t="shared" si="7"/>
+        <v>8.1928538464887526E-2</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2192,23 +3380,56 @@
       <c r="C38">
         <v>838669.82</v>
       </c>
-      <c r="E38" s="5"/>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>16630.180000000051</v>
+      </c>
+      <c r="E38" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9443680579913542E-2</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
       <c r="G38">
         <v>792800</v>
       </c>
       <c r="H38">
         <v>753451.96</v>
       </c>
-      <c r="J38" s="5"/>
+      <c r="I38">
+        <f t="shared" si="3"/>
+        <v>39348.040000000037</v>
+      </c>
+      <c r="J38" s="5">
+        <f t="shared" si="4"/>
+        <v>4.9631735620585316E-2</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
       <c r="L38">
         <v>777800</v>
       </c>
       <c r="M38">
         <v>777663.26</v>
       </c>
-      <c r="O38" s="5"/>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="N38">
+        <f t="shared" si="6"/>
+        <v>136.73999999999069</v>
+      </c>
+      <c r="O38" s="5">
+        <f t="shared" si="7"/>
+        <v>1.7580354847003174E-4</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -2218,23 +3439,56 @@
       <c r="C39">
         <v>813108.87</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>70791.13</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" si="1"/>
+        <v>8.008952370177623E-2</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="G39">
         <v>1294400</v>
       </c>
       <c r="H39">
         <v>1114242.27999999</v>
       </c>
-      <c r="J39" s="5"/>
+      <c r="I39">
+        <f t="shared" si="3"/>
+        <v>180157.72000000998</v>
+      </c>
+      <c r="J39" s="5">
+        <f t="shared" si="4"/>
+        <v>0.13918241656366656</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
       <c r="L39">
         <v>1759500</v>
       </c>
       <c r="M39">
         <v>1680463.8699999901</v>
       </c>
-      <c r="O39" s="5"/>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="N39">
+        <f t="shared" si="6"/>
+        <v>79036.1300000099</v>
+      </c>
+      <c r="O39" s="5">
+        <f t="shared" si="7"/>
+        <v>4.4919653310605226E-2</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2244,23 +3498,56 @@
       <c r="C40">
         <v>37565141.859999903</v>
       </c>
-      <c r="E40" s="5"/>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>816758.14000009745</v>
+      </c>
+      <c r="E40" s="5">
+        <f t="shared" si="1"/>
+        <v>2.1279773539092578E-2</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
       <c r="G40">
         <v>39964900</v>
       </c>
       <c r="H40">
         <v>38095240.189999901</v>
       </c>
-      <c r="J40" s="5"/>
+      <c r="I40">
+        <f t="shared" si="3"/>
+        <v>1869659.8100000992</v>
+      </c>
+      <c r="J40" s="5">
+        <f t="shared" si="4"/>
+        <v>4.6782546934937892E-2</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
       <c r="L40">
         <v>40216700</v>
       </c>
       <c r="M40">
         <v>39606263.709999897</v>
       </c>
-      <c r="O40" s="5"/>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="N40">
+        <f t="shared" si="6"/>
+        <v>610436.29000010341</v>
+      </c>
+      <c r="O40" s="5">
+        <f t="shared" si="7"/>
+        <v>1.5178676768608648E-2</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2270,23 +3557,56 @@
       <c r="C41">
         <v>4409060.2099999897</v>
       </c>
-      <c r="E41" s="5"/>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>184239.79000001028</v>
+      </c>
+      <c r="E41" s="5">
+        <f t="shared" si="1"/>
+        <v>4.0110550149132493E-2</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="G41">
         <v>5089500</v>
       </c>
       <c r="H41">
         <v>4956043.6699999897</v>
       </c>
-      <c r="J41" s="5"/>
+      <c r="I41">
+        <f t="shared" si="3"/>
+        <v>133456.33000001032</v>
+      </c>
+      <c r="J41" s="5">
+        <f t="shared" si="4"/>
+        <v>2.6221894095689226E-2</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
       <c r="L41">
         <v>4799900</v>
       </c>
       <c r="M41">
         <v>4717822.6500000004</v>
       </c>
-      <c r="O41" s="5"/>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="N41">
+        <f t="shared" si="6"/>
+        <v>82077.349999999627</v>
+      </c>
+      <c r="O41" s="5">
+        <f t="shared" si="7"/>
+        <v>1.7099804162586642E-2</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2296,23 +3616,56 @@
       <c r="C42">
         <v>188551675.67999899</v>
       </c>
-      <c r="E42" s="5"/>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>41624.320001006126</v>
+      </c>
+      <c r="E42" s="5">
+        <f t="shared" si="1"/>
+        <v>2.2070943135841053E-4</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
       <c r="G42">
         <v>199130300</v>
       </c>
       <c r="H42">
         <v>196755033.31</v>
       </c>
-      <c r="J42" s="5"/>
+      <c r="I42">
+        <f t="shared" si="3"/>
+        <v>2375266.6899999976</v>
+      </c>
+      <c r="J42" s="5">
+        <f t="shared" si="4"/>
+        <v>1.1928203241796942E-2</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
       <c r="L42">
         <v>199954600</v>
       </c>
       <c r="M42">
         <v>199954563.74999899</v>
       </c>
-      <c r="O42" s="5"/>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="N42">
+        <f t="shared" si="6"/>
+        <v>36.250001013278961</v>
+      </c>
+      <c r="O42" s="5">
+        <f t="shared" si="7"/>
+        <v>1.8129115815929696E-7</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -2322,23 +3675,56 @@
       <c r="C43">
         <v>7968645.8300000001</v>
       </c>
-      <c r="E43" s="5"/>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>166754.16999999993</v>
+      </c>
+      <c r="E43" s="5">
+        <f t="shared" si="1"/>
+        <v>2.0497353541313264E-2</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
       <c r="G43">
         <v>8560800</v>
       </c>
       <c r="H43">
         <v>8171472.0199999996</v>
       </c>
-      <c r="J43" s="5"/>
+      <c r="I43">
+        <f t="shared" si="3"/>
+        <v>389327.98000000045</v>
+      </c>
+      <c r="J43" s="5">
+        <f t="shared" si="4"/>
+        <v>4.5477990374731388E-2</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
       <c r="L43">
         <v>8497500</v>
       </c>
       <c r="M43">
         <v>8150982.5699999901</v>
       </c>
-      <c r="O43" s="5"/>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="N43">
+        <f t="shared" si="6"/>
+        <v>346517.43000000995</v>
+      </c>
+      <c r="O43" s="5">
+        <f t="shared" si="7"/>
+        <v>4.0778750220654303E-2</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2348,23 +3734,56 @@
       <c r="C44">
         <v>29789104.379999999</v>
       </c>
-      <c r="E44" s="5"/>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>294095.62000000104</v>
+      </c>
+      <c r="E44" s="5">
+        <f t="shared" si="1"/>
+        <v>9.7760750186150751E-3</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
       <c r="G44">
         <v>31040700</v>
       </c>
       <c r="H44">
         <v>30793711.48</v>
       </c>
-      <c r="J44" s="5"/>
+      <c r="I44">
+        <f t="shared" si="3"/>
+        <v>246988.51999999955</v>
+      </c>
+      <c r="J44" s="5">
+        <f t="shared" si="4"/>
+        <v>7.9569249404813532E-3</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
       <c r="L44">
         <v>31282200</v>
       </c>
       <c r="M44">
         <v>31282141.25</v>
       </c>
-      <c r="O44" s="5"/>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="N44">
+        <f t="shared" si="6"/>
+        <v>58.75</v>
+      </c>
+      <c r="O44" s="5">
+        <f t="shared" si="7"/>
+        <v>1.8780648419868168E-6</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2374,23 +3793,56 @@
       <c r="C45">
         <v>54589584.0499999</v>
       </c>
-      <c r="E45" s="5"/>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>712015.95000009984</v>
+      </c>
+      <c r="E45" s="5">
+        <f t="shared" si="1"/>
+        <v>1.287514194887851E-2</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
       <c r="G45">
         <v>56792200</v>
       </c>
       <c r="H45">
         <v>54594953.959999897</v>
       </c>
-      <c r="J45" s="5"/>
+      <c r="I45">
+        <f t="shared" si="3"/>
+        <v>2197246.0400001034</v>
+      </c>
+      <c r="J45" s="5">
+        <f t="shared" si="4"/>
+        <v>3.8689222111488959E-2</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
       <c r="L45">
         <v>56027100</v>
       </c>
       <c r="M45">
         <v>55386549.6599999</v>
       </c>
-      <c r="O45" s="5"/>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="N45">
+        <f t="shared" si="6"/>
+        <v>640550.34000010043</v>
+      </c>
+      <c r="O45" s="5">
+        <f t="shared" si="7"/>
+        <v>1.1432866237947358E-2</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -2400,23 +3852,56 @@
       <c r="C46">
         <v>258322.43</v>
       </c>
-      <c r="E46" s="5"/>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>777.57000000000698</v>
+      </c>
+      <c r="E46" s="5">
+        <f t="shared" si="1"/>
+        <v>3.0010420686993711E-3</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
       <c r="G46">
         <v>266000</v>
       </c>
       <c r="H46">
         <v>257402.90999999901</v>
       </c>
-      <c r="J46" s="5"/>
+      <c r="I46">
+        <f t="shared" si="3"/>
+        <v>8597.090000000986</v>
+      </c>
+      <c r="J46" s="5">
+        <f t="shared" si="4"/>
+        <v>3.2319887218048821E-2</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
       <c r="L46">
         <v>267100</v>
       </c>
       <c r="M46">
         <v>254753.15999999901</v>
       </c>
-      <c r="O46" s="5"/>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="N46">
+        <f t="shared" si="6"/>
+        <v>12346.840000000986</v>
+      </c>
+      <c r="O46" s="5">
+        <f t="shared" si="7"/>
+        <v>4.6225533508053113E-2</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -2426,23 +3911,56 @@
       <c r="C47">
         <v>70378426.719999999</v>
       </c>
-      <c r="E47" s="5"/>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>12273.280000001192</v>
+      </c>
+      <c r="E47" s="5">
+        <f t="shared" si="1"/>
+        <v>1.7435939690898361E-4</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
       <c r="G47">
         <v>73467000</v>
       </c>
       <c r="H47">
         <v>73442541.659999996</v>
       </c>
-      <c r="J47" s="5"/>
+      <c r="I47">
+        <f t="shared" si="3"/>
+        <v>24458.340000003576</v>
+      </c>
+      <c r="J47" s="5">
+        <f t="shared" si="4"/>
+        <v>3.3291600310348285E-4</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
       <c r="L47">
         <v>75072800</v>
       </c>
       <c r="M47">
         <v>75050829.179999903</v>
       </c>
-      <c r="O47" s="5"/>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="N47">
+        <f t="shared" si="6"/>
+        <v>21970.820000097156</v>
+      </c>
+      <c r="O47" s="5">
+        <f t="shared" si="7"/>
+        <v>2.9266019117572752E-4</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -2452,23 +3970,56 @@
       <c r="C48">
         <v>6527352.5699999901</v>
       </c>
-      <c r="E48" s="5"/>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>209747.43000000995</v>
+      </c>
+      <c r="E48" s="5">
+        <f t="shared" si="1"/>
+        <v>3.1133192323107857E-2</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="G48">
         <v>7214700</v>
       </c>
       <c r="H48">
         <v>6922072.5599999996</v>
       </c>
-      <c r="J48" s="5"/>
+      <c r="I48">
+        <f t="shared" si="3"/>
+        <v>292627.44000000041</v>
+      </c>
+      <c r="J48" s="5">
+        <f t="shared" si="4"/>
+        <v>4.0559890224125802E-2</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
       <c r="L48">
         <v>7289800</v>
       </c>
       <c r="M48">
         <v>6882350.23999999</v>
       </c>
-      <c r="O48" s="5"/>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="N48">
+        <f t="shared" si="6"/>
+        <v>407449.76000001002</v>
+      </c>
+      <c r="O48" s="5">
+        <f t="shared" si="7"/>
+        <v>5.5893132870587676E-2</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -2478,23 +4029,56 @@
       <c r="C49">
         <v>90499.43</v>
       </c>
-      <c r="E49" s="5"/>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>1700.570000000007</v>
+      </c>
+      <c r="E49" s="5">
+        <f t="shared" si="1"/>
+        <v>1.8444360086767971E-2</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="G49">
         <v>102600</v>
       </c>
       <c r="H49">
         <v>95466.880000000005</v>
       </c>
-      <c r="J49" s="5"/>
+      <c r="I49">
+        <f t="shared" si="3"/>
+        <v>7133.1199999999953</v>
+      </c>
+      <c r="J49" s="5">
+        <f t="shared" si="4"/>
+        <v>6.9523586744639335E-2</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
       <c r="L49">
         <v>0</v>
       </c>
       <c r="M49">
         <v>0</v>
       </c>
-      <c r="O49" s="5"/>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="N49">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O49" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -2504,23 +4088,56 @@
       <c r="C50">
         <v>832600</v>
       </c>
-      <c r="E50" s="5"/>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E50" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
       <c r="G50">
         <v>859100</v>
       </c>
       <c r="H50">
         <v>859100</v>
       </c>
-      <c r="J50" s="5"/>
+      <c r="I50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
       <c r="L50">
         <v>843200</v>
       </c>
       <c r="M50">
         <v>843200</v>
       </c>
-      <c r="O50" s="5"/>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="N50">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O50" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -2530,23 +4147,56 @@
       <c r="C51">
         <v>8499425.3399999905</v>
       </c>
-      <c r="E51" s="5"/>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>110074.66000000946</v>
+      </c>
+      <c r="E51" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2785255822058129E-2</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="G51">
         <v>8925500</v>
       </c>
       <c r="H51">
         <v>8599059.6199999992</v>
       </c>
-      <c r="J51" s="5"/>
+      <c r="I51">
+        <f t="shared" si="3"/>
+        <v>326440.38000000082</v>
+      </c>
+      <c r="J51" s="5">
+        <f t="shared" si="4"/>
+        <v>3.6573903982970231E-2</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
       <c r="L51">
         <v>8833900</v>
       </c>
       <c r="M51">
         <v>8735843.3100000005</v>
       </c>
-      <c r="O51" s="5"/>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="N51">
+        <f t="shared" si="6"/>
+        <v>98056.689999999478</v>
+      </c>
+      <c r="O51" s="5">
+        <f t="shared" si="7"/>
+        <v>1.1100045280114048E-2</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -2556,28 +4206,61 @@
       <c r="C52">
         <v>2254684.7999999998</v>
       </c>
-      <c r="E52" s="5"/>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>196315.20000000019</v>
+      </c>
+      <c r="E52" s="5">
+        <f t="shared" si="1"/>
+        <v>8.009596083231342E-2</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="G52">
         <v>2440700</v>
       </c>
       <c r="H52">
         <v>2204672.88</v>
       </c>
-      <c r="J52" s="5"/>
+      <c r="I52">
+        <f t="shared" si="3"/>
+        <v>236027.12000000011</v>
+      </c>
+      <c r="J52" s="5">
+        <f t="shared" si="4"/>
+        <v>9.6704683082722218E-2</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
       <c r="L52">
         <v>2321600</v>
       </c>
       <c r="M52">
         <v>2056835.26</v>
       </c>
-      <c r="O52" s="5"/>
-    </row>
-    <row r="54" spans="1:15" ht="15">
+      <c r="N52">
+        <f t="shared" si="6"/>
+        <v>264764.74</v>
+      </c>
+      <c r="O52" s="5">
+        <f t="shared" si="7"/>
+        <v>0.11404408166781529</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -2591,42 +4274,114 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="57" spans="1:15">
+      <c r="B56">
+        <f>VLOOKUP($A$56,$A2:$P52,4,FALSE)</f>
+        <v>36209.630000000005</v>
+      </c>
+      <c r="C56">
+        <f>VLOOKUP($A$56,$A2:$P52,9,FALSE)</f>
+        <v>27292.159999999974</v>
+      </c>
+      <c r="D56">
+        <f>VLOOKUP($A$56,$A2:$P52,14,FALSE)</f>
+        <v>9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="B57">
+        <f>VLOOKUP($A$57,$A2:$P52,4,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <f>VLOOKUP($A$57,$A2:$P52,9,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <f>VLOOKUP($A$57,$A2:$P52,14,FALSE)</f>
+        <v>311228.08999999997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="B58">
+        <f>VLOOKUP($A$58,$A2:$P52,4,FALSE)</f>
+        <v>149396.10000000987</v>
+      </c>
+      <c r="C58">
+        <f>VLOOKUP($A$58,$A2:$P52,9,FALSE)</f>
+        <v>189254.06000000006</v>
+      </c>
+      <c r="D58">
+        <f>VLOOKUP($A$58,$A2:$P52,14,FALSE)</f>
+        <v>374962.91000000015</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="60" spans="1:15">
+      <c r="B59">
+        <f>VLOOKUP($A$59,$A2:$P52,4,FALSE)</f>
+        <v>12230.810000000056</v>
+      </c>
+      <c r="C59">
+        <f>VLOOKUP($A$59,$A2:$P52,9,FALSE)</f>
+        <v>45485.580000000075</v>
+      </c>
+      <c r="D59">
+        <f>VLOOKUP($A$59,$A2:$P52,14,FALSE)</f>
+        <v>72.879999999888241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="61" spans="1:15">
+      <c r="B60">
+        <f>VLOOKUP($A$60,$A2:$P52,4,FALSE)</f>
+        <v>4950.4699999999721</v>
+      </c>
+      <c r="C60">
+        <f>VLOOKUP($A$60,$A2:$P52,9,FALSE)</f>
+        <v>8005.7900000010268</v>
+      </c>
+      <c r="D60">
+        <f>VLOOKUP($A$60,$A2:$P52,14,FALSE)</f>
+        <v>1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" ht="15">
+      <c r="B61">
+        <f>VLOOKUP($A$61,$A2:$P52,4,FALSE)</f>
+        <v>184239.79000001028</v>
+      </c>
+      <c r="C61">
+        <f>VLOOKUP($A$61,$A2:$P52,9,FALSE)</f>
+        <v>133456.33000001032</v>
+      </c>
+      <c r="D61">
+        <f>VLOOKUP($A$61,$A2:$P52,14,FALSE)</f>
+        <v>82077.349999999627</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -2640,43 +4395,114 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="15">
+      <c r="B65">
+        <f>_xlfn.XLOOKUP(A65,A2:A52,D2:D52)</f>
+        <v>36209.630000000005</v>
+      </c>
+      <c r="C65">
+        <f>_xlfn.XLOOKUP(A65,A2:A52,I2:I52)</f>
+        <v>27292.159999999974</v>
+      </c>
+      <c r="D65">
+        <f>_xlfn.XLOOKUP(A65,A2:A52,N2:N52)</f>
+        <v>9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="15">
+      <c r="B66">
+        <f t="shared" ref="B66:B70" si="9">_xlfn.XLOOKUP(A66,A3:A53,D3:D53)</f>
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ref="C66:C70" si="10">_xlfn.XLOOKUP(A66,A3:A53,I3:I53)</f>
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <f t="shared" ref="D66:D70" si="11">_xlfn.XLOOKUP(A66,A3:A53,N3:N53)</f>
+        <v>311228.08999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="B67">
+        <f t="shared" si="9"/>
+        <v>149396.10000000987</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="10"/>
+        <v>189254.06000000006</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="11"/>
+        <v>374962.91000000015</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="B68">
+        <f t="shared" si="9"/>
+        <v>12230.810000000056</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="10"/>
+        <v>45485.580000000075</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="11"/>
+        <v>72.879999999888241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="B69">
+        <f t="shared" si="9"/>
+        <v>4950.4699999999721</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="10"/>
+        <v>8005.7900000010268</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="11"/>
+        <v>1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="15"/>
-    <row r="72" spans="1:4" ht="15">
+      <c r="B70">
+        <f t="shared" si="9"/>
+        <v>184239.79000001028</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="10"/>
+        <v>133456.33000001032</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="11"/>
+        <v>82077.349999999627</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -2690,48 +4516,119 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="15">
+      <c r="B74">
+        <f>INDEX(D2:D52,MATCH(A74,A2:A52,0))</f>
+        <v>36209.630000000005</v>
+      </c>
+      <c r="C74">
+        <f>INDEX(I2:I52,MATCH(A74,A2:A52,0))</f>
+        <v>27292.159999999974</v>
+      </c>
+      <c r="D74">
+        <f>INDEX(N2:N52,MATCH(A74,A2:A52,0))</f>
+        <v>9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="B75">
+        <f t="shared" ref="B75:B79" si="12">INDEX(D3:D53,MATCH(A75,A3:A53,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <f t="shared" ref="C75:C79" si="13">INDEX(I3:I53,MATCH(A75,A3:A53,0))</f>
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ref="D75:D79" si="14">INDEX(N3:N53,MATCH(A75,A3:A53,0))</f>
+        <v>311228.08999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="B76">
+        <f t="shared" si="12"/>
+        <v>149396.10000000987</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="13"/>
+        <v>189254.06000000006</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="14"/>
+        <v>374962.91000000015</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="B77">
+        <f t="shared" si="12"/>
+        <v>12230.810000000056</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="13"/>
+        <v>45485.580000000075</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="14"/>
+        <v>72.879999999888241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="B78">
+        <f t="shared" si="12"/>
+        <v>4950.4699999999721</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="13"/>
+        <v>8005.7900000010268</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="14"/>
+        <v>1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="15"/>
-    <row r="81" spans="1:7" ht="15">
+      <c r="B79">
+        <f t="shared" si="12"/>
+        <v>184239.79000001028</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="13"/>
+        <v>133456.33000001032</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="14"/>
+        <v>82077.349999999627</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>71</v>
       </c>
@@ -2739,34 +4636,33 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>73</v>
       </c>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>74</v>
       </c>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>75</v>
       </c>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
     </row>
-    <row r="87" spans="1:7" ht="15"/>
-    <row r="88" spans="1:7" ht="15">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -2782,7 +4678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
         <v>0</v>
       </c>
@@ -2802,7 +4698,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>73</v>
       </c>
@@ -2810,7 +4706,7 @@
       <c r="E91" s="5"/>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>74</v>
       </c>
@@ -2818,7 +4714,7 @@
       <c r="E92" s="5"/>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>75</v>
       </c>
@@ -2826,12 +4722,12 @@
       <c r="E93" s="5"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="95" spans="1:7" ht="15">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>77</v>
       </c>
@@ -2847,7 +4743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B97" s="8" t="s">
         <v>0</v>
       </c>
@@ -2867,7 +4763,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>73</v>
       </c>
@@ -2876,7 +4772,7 @@
       <c r="G98" s="4"/>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -2885,7 +4781,7 @@
       <c r="G99" s="4"/>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>75</v>
       </c>
@@ -2894,12 +4790,6 @@
       <c r="G100" s="4"/>
       <c r="I100" s="4"/>
     </row>
-    <row r="102" spans="1:9" ht="15"/>
-    <row r="103" spans="1:9" ht="15"/>
-    <row r="104" spans="1:9" ht="15"/>
-    <row r="105" spans="1:9" ht="15"/>
-    <row r="106" spans="1:9" ht="15"/>
-    <row r="107" spans="1:9" ht="15"/>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
@@ -2919,13 +4809,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2933,7 +4823,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2941,7 +4831,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2949,7 +4839,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2957,7 +4847,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2965,7 +4855,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2973,7 +4863,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2981,7 +4871,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -2989,7 +4879,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -2997,7 +4887,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>